<commit_message>
w9 complete w6 assignments marked and returned (except for a couple of EC)
</commit_message>
<xml_diff>
--- a/admin/LIN6209 student data.xlsx
+++ b/admin/LIN6209 student data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/138e04b35f3df159/AllTeaching/_QMUL/LIN6209/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/138e04b35f3df159/AllTeaching/_QMUL/LIN6209/admin/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="490" documentId="8_{D4084AF5-A7E0-4A89-8908-66192E3C3F85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{647AC267-8963-4137-B538-A10BFB661B2D}"/>
+  <xr:revisionPtr revIDLastSave="655" documentId="8_{D4084AF5-A7E0-4A89-8908-66192E3C3F85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ED532B37-0EDE-4144-A464-E414EC704DCA}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21820" xr2:uid="{FBA493EA-9E30-4955-99CC-D2245AEE8977}"/>
   </bookViews>
@@ -16,7 +16,8 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$2:$Q$21</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$2:$AF$21</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="0">Sheet1!$A:$A</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="87">
   <si>
     <t>F</t>
   </si>
@@ -274,16 +275,31 @@
     <t>P withdrew</t>
   </si>
   <si>
-    <t>#</t>
-  </si>
-  <si>
-    <t>18/19</t>
-  </si>
-  <si>
     <t>Lin6209 Coding for Linguists</t>
   </si>
   <si>
     <t>I</t>
+  </si>
+  <si>
+    <t>Attendance</t>
+  </si>
+  <si>
+    <t>Assignments</t>
+  </si>
+  <si>
+    <t>18/10</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>*</t>
+  </si>
+  <si>
+    <t>*24th</t>
+  </si>
+  <si>
+    <t>**</t>
   </si>
 </sst>
 </file>
@@ -293,7 +309,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -331,6 +347,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -350,7 +373,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="29">
+  <borders count="41">
     <border>
       <left/>
       <right/>
@@ -730,14 +753,157 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFFF0000"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FFFF0000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FFFF0000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFFF0000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFFF0000"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FFFF0000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFFF0000"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FFFF0000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFFF0000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFFF0000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFFF0000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFFF0000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFFF0000"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FFFF0000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color rgb="FFFF0000"/>
+      </left>
+      <right style="thick">
+        <color rgb="FFFF0000"/>
+      </right>
+      <top style="thick">
+        <color rgb="FFFF0000"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="FFFF0000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="74">
+  <cellXfs count="101">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -908,12 +1074,80 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="2" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="3" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="2" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="3" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="2" borderId="4" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="2" borderId="1" xfId="4" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="2" borderId="1" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="3" borderId="1" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="2" borderId="4" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="2" borderId="29" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="2" borderId="30" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="2" borderId="31" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="32" xfId="2" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="33" xfId="2" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="34" xfId="2" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="35" xfId="2" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="36" xfId="2" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="37" xfId="2" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="38" xfId="2" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="3" fillId="2" borderId="39" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="3" borderId="30" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="2" borderId="40" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="5">
     <cellStyle name="Good" xfId="2" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Neutral" xfId="3" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="4" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1323,13 +1557,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0BFC96F-D0A0-4D45-84C2-1CEA6D400A83}">
-  <sheetPr codeName="Sheet1">
-    <pageSetUpPr fitToPage="1"/>
-  </sheetPr>
-  <dimension ref="A2:CZ41"/>
+  <sheetPr codeName="Sheet1"/>
+  <dimension ref="A1:CZ41"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="Z5" sqref="Z5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1339,15 +1572,24 @@
     <col min="3" max="3" width="29.36328125" customWidth="1"/>
     <col min="4" max="5" width="1.6328125" customWidth="1"/>
     <col min="6" max="17" width="5.6328125" customWidth="1"/>
+    <col min="18" max="18" width="8.7265625" style="75"/>
     <col min="19" max="19" width="8.81640625" style="1" bestFit="1" customWidth="1"/>
     <col min="20" max="32" width="5.6328125" customWidth="1"/>
     <col min="33" max="33" width="10.54296875" style="58" customWidth="1"/>
     <col min="34" max="104" width="8.7265625" style="58"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:104" x14ac:dyDescent="0.35">
+      <c r="F1" t="s">
+        <v>80</v>
+      </c>
+      <c r="T1" t="s">
+        <v>81</v>
+      </c>
+    </row>
     <row r="2" spans="1:104" ht="21.5" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="F2" s="73">
         <v>44466</v>
@@ -1359,7 +1601,7 @@
         <v>44480</v>
       </c>
       <c r="I2" s="73" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="J2" s="73">
         <v>44494</v>
@@ -1486,7 +1728,9 @@
       <c r="C4" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="F4" s="63"/>
+      <c r="F4" s="63" t="s">
+        <v>74</v>
+      </c>
       <c r="G4" s="35" t="s">
         <v>74</v>
       </c>
@@ -1499,13 +1743,23 @@
       <c r="J4" s="35" t="s">
         <v>74</v>
       </c>
-      <c r="K4" s="35"/>
-      <c r="L4" s="35"/>
-      <c r="M4" s="35"/>
+      <c r="K4" s="35" t="s">
+        <v>74</v>
+      </c>
+      <c r="L4" s="74" t="s">
+        <v>83</v>
+      </c>
+      <c r="M4" s="35" t="s">
+        <v>74</v>
+      </c>
       <c r="N4" s="35"/>
       <c r="O4" s="35"/>
       <c r="P4" s="35"/>
       <c r="Q4" s="36"/>
+      <c r="R4" s="76">
+        <f>COUNTIFS(F4:Q4, "P")+COUNTIFS(F4:Q4, "O")</f>
+        <v>7</v>
+      </c>
       <c r="S4" s="33" t="s">
         <v>0</v>
       </c>
@@ -1515,11 +1769,19 @@
       <c r="U4" s="35">
         <v>11</v>
       </c>
-      <c r="V4" s="35"/>
-      <c r="W4" s="35"/>
-      <c r="X4" s="35"/>
-      <c r="Y4" s="35"/>
-      <c r="Z4" s="35"/>
+      <c r="V4" s="80">
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="W4" s="84"/>
+      <c r="X4" s="80">
+        <f>4.75/8</f>
+        <v>0.59375</v>
+      </c>
+      <c r="Y4" s="84"/>
+      <c r="Z4" s="80">
+        <f>13.25/18</f>
+        <v>0.73611111111111116</v>
+      </c>
       <c r="AA4" s="35"/>
       <c r="AB4" s="35"/>
       <c r="AC4" s="35"/>
@@ -1609,7 +1871,9 @@
       <c r="C5" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="63"/>
+      <c r="F5" s="63" t="s">
+        <v>74</v>
+      </c>
       <c r="G5" s="35" t="s">
         <v>74</v>
       </c>
@@ -1623,14 +1887,17 @@
         <v>74</v>
       </c>
       <c r="K5" s="35"/>
-      <c r="L5" s="35"/>
+      <c r="L5" s="74" t="s">
+        <v>83</v>
+      </c>
       <c r="M5" s="35"/>
       <c r="N5" s="35"/>
       <c r="O5" s="35"/>
       <c r="P5" s="35"/>
       <c r="Q5" s="36"/>
-      <c r="R5" s="32" t="s">
-        <v>78</v>
+      <c r="R5" s="76">
+        <f t="shared" ref="R5:R20" si="0">COUNTIFS(F5:Q5, "P")+COUNTIFS(F5:Q5, "O")</f>
+        <v>5</v>
       </c>
       <c r="S5" s="33" t="s">
         <v>70</v>
@@ -1639,11 +1906,18 @@
         <v>1</v>
       </c>
       <c r="U5" s="35"/>
-      <c r="V5" s="35"/>
-      <c r="W5" s="35"/>
-      <c r="X5" s="35"/>
-      <c r="Y5" s="35"/>
-      <c r="Z5" s="35"/>
+      <c r="V5" s="80">
+        <f>9/12</f>
+        <v>0.75</v>
+      </c>
+      <c r="W5" s="84"/>
+      <c r="X5" s="80" t="s">
+        <v>85</v>
+      </c>
+      <c r="Y5" s="84"/>
+      <c r="Z5" s="83" t="s">
+        <v>84</v>
+      </c>
       <c r="AA5" s="35"/>
       <c r="AB5" s="35"/>
       <c r="AC5" s="35"/>
@@ -1733,7 +2007,9 @@
       <c r="C6" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="F6" s="63"/>
+      <c r="F6" s="63" t="s">
+        <v>74</v>
+      </c>
       <c r="G6" s="35" t="s">
         <v>74</v>
       </c>
@@ -1746,13 +2022,23 @@
       <c r="J6" s="35">
         <v>0</v>
       </c>
-      <c r="K6" s="35"/>
-      <c r="L6" s="35"/>
-      <c r="M6" s="35"/>
+      <c r="K6" s="35" t="s">
+        <v>74</v>
+      </c>
+      <c r="L6" s="35" t="s">
+        <v>83</v>
+      </c>
+      <c r="M6" s="35" t="s">
+        <v>75</v>
+      </c>
       <c r="N6" s="35"/>
       <c r="O6" s="35"/>
       <c r="P6" s="35"/>
       <c r="Q6" s="36"/>
+      <c r="R6" s="76">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
       <c r="S6" s="33"/>
       <c r="T6" s="34" t="s">
         <v>1</v>
@@ -1760,11 +2046,18 @@
       <c r="U6" s="35">
         <v>3</v>
       </c>
-      <c r="V6" s="35"/>
-      <c r="W6" s="35"/>
-      <c r="X6" s="35"/>
-      <c r="Y6" s="35"/>
-      <c r="Z6" s="35"/>
+      <c r="V6" s="80">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="W6" s="84"/>
+      <c r="X6" s="80">
+        <v>0.625</v>
+      </c>
+      <c r="Y6" s="84"/>
+      <c r="Z6" s="80">
+        <f>15.5/18</f>
+        <v>0.86111111111111116</v>
+      </c>
       <c r="AA6" s="35"/>
       <c r="AB6" s="35"/>
       <c r="AC6" s="35"/>
@@ -1854,7 +2147,9 @@
       <c r="C7" s="31" t="s">
         <v>19</v>
       </c>
-      <c r="F7" s="63"/>
+      <c r="F7" s="63" t="s">
+        <v>74</v>
+      </c>
       <c r="G7" s="35" t="s">
         <v>74</v>
       </c>
@@ -1862,16 +2157,22 @@
         <v>74</v>
       </c>
       <c r="I7" s="35" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="J7" s="35"/>
       <c r="K7" s="35"/>
-      <c r="L7" s="35"/>
+      <c r="L7" s="35" t="s">
+        <v>83</v>
+      </c>
       <c r="M7" s="35"/>
       <c r="N7" s="35"/>
       <c r="O7" s="35"/>
       <c r="P7" s="35"/>
       <c r="Q7" s="36"/>
+      <c r="R7" s="76">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
       <c r="S7" s="33" t="s">
         <v>70</v>
       </c>
@@ -1879,11 +2180,19 @@
       <c r="U7" s="35">
         <v>6</v>
       </c>
-      <c r="V7" s="35"/>
-      <c r="W7" s="35"/>
-      <c r="X7" s="35"/>
-      <c r="Y7" s="35"/>
-      <c r="Z7" s="35"/>
+      <c r="V7" s="80">
+        <f>10.3/12</f>
+        <v>0.85833333333333339</v>
+      </c>
+      <c r="W7" s="84"/>
+      <c r="X7" s="80">
+        <f>7.5/8</f>
+        <v>0.9375</v>
+      </c>
+      <c r="Y7" s="84"/>
+      <c r="Z7" s="83" t="s">
+        <v>86</v>
+      </c>
       <c r="AA7" s="35"/>
       <c r="AB7" s="35"/>
       <c r="AC7" s="35"/>
@@ -1973,7 +2282,9 @@
       <c r="C8" s="31" t="s">
         <v>23</v>
       </c>
-      <c r="F8" s="63"/>
+      <c r="F8" s="63" t="s">
+        <v>74</v>
+      </c>
       <c r="G8" s="35" t="s">
         <v>74</v>
       </c>
@@ -1986,15 +2297,22 @@
       <c r="J8" s="35" t="s">
         <v>74</v>
       </c>
-      <c r="K8" s="35"/>
-      <c r="L8" s="35"/>
-      <c r="M8" s="35"/>
+      <c r="K8" s="35" t="s">
+        <v>74</v>
+      </c>
+      <c r="L8" s="35" t="s">
+        <v>83</v>
+      </c>
+      <c r="M8" s="35" t="s">
+        <v>74</v>
+      </c>
       <c r="N8" s="35"/>
       <c r="O8" s="35"/>
       <c r="P8" s="35"/>
       <c r="Q8" s="36"/>
-      <c r="R8" s="32" t="s">
-        <v>78</v>
+      <c r="R8" s="76">
+        <f t="shared" si="0"/>
+        <v>7</v>
       </c>
       <c r="S8" s="33"/>
       <c r="T8" s="34" t="s">
@@ -2003,11 +2321,18 @@
       <c r="U8" s="35">
         <v>9</v>
       </c>
-      <c r="V8" s="35"/>
-      <c r="W8" s="35"/>
-      <c r="X8" s="35"/>
-      <c r="Y8" s="35"/>
-      <c r="Z8" s="35"/>
+      <c r="V8" s="80">
+        <v>1</v>
+      </c>
+      <c r="W8" s="84"/>
+      <c r="X8" s="80">
+        <v>0.875</v>
+      </c>
+      <c r="Y8" s="84"/>
+      <c r="Z8" s="80">
+        <f>14.75/18</f>
+        <v>0.81944444444444442</v>
+      </c>
       <c r="AA8" s="35"/>
       <c r="AB8" s="35"/>
       <c r="AC8" s="35"/>
@@ -2018,8 +2343,8 @@
       <c r="AH8" s="59"/>
       <c r="AI8" s="59"/>
       <c r="AJ8" s="59"/>
-      <c r="AK8" s="59"/>
-      <c r="AL8" s="59"/>
+      <c r="AK8" s="90"/>
+      <c r="AL8" s="91"/>
       <c r="AM8" s="59"/>
       <c r="AN8" s="59"/>
       <c r="AO8" s="59"/>
@@ -2097,7 +2422,9 @@
       <c r="C9" s="31" t="s">
         <v>25</v>
       </c>
-      <c r="F9" s="63"/>
+      <c r="F9" s="63" t="s">
+        <v>74</v>
+      </c>
       <c r="G9" s="35" t="s">
         <v>74</v>
       </c>
@@ -2107,12 +2434,18 @@
       </c>
       <c r="J9" s="35"/>
       <c r="K9" s="35"/>
-      <c r="L9" s="35"/>
+      <c r="L9" s="35" t="s">
+        <v>83</v>
+      </c>
       <c r="M9" s="35"/>
       <c r="N9" s="35"/>
       <c r="O9" s="35"/>
       <c r="P9" s="35"/>
       <c r="Q9" s="36"/>
+      <c r="R9" s="76">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
       <c r="S9" s="33"/>
       <c r="T9" s="34" t="s">
         <v>1</v>
@@ -2120,11 +2453,19 @@
       <c r="U9" s="35">
         <v>11</v>
       </c>
-      <c r="V9" s="35"/>
-      <c r="W9" s="35"/>
-      <c r="X9" s="35"/>
-      <c r="Y9" s="35"/>
-      <c r="Z9" s="35"/>
+      <c r="V9" s="80">
+        <f>11/12</f>
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="W9" s="84"/>
+      <c r="X9" s="80">
+        <v>0.875</v>
+      </c>
+      <c r="Y9" s="84"/>
+      <c r="Z9" s="80">
+        <f>17.75/19</f>
+        <v>0.93421052631578949</v>
+      </c>
       <c r="AA9" s="35"/>
       <c r="AB9" s="35"/>
       <c r="AC9" s="35"/>
@@ -2135,8 +2476,8 @@
       <c r="AH9" s="59"/>
       <c r="AI9" s="59"/>
       <c r="AJ9" s="59"/>
-      <c r="AK9" s="59"/>
-      <c r="AL9" s="59"/>
+      <c r="AK9" s="92"/>
+      <c r="AL9" s="93"/>
       <c r="AM9" s="59"/>
       <c r="AN9" s="59"/>
       <c r="AO9" s="59"/>
@@ -2214,7 +2555,9 @@
       <c r="C10" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="F10" s="63"/>
+      <c r="F10" s="63" t="s">
+        <v>75</v>
+      </c>
       <c r="G10" s="35" t="s">
         <v>75</v>
       </c>
@@ -2225,15 +2568,20 @@
       <c r="J10" s="35" t="s">
         <v>75</v>
       </c>
-      <c r="K10" s="35"/>
-      <c r="L10" s="35"/>
+      <c r="K10" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="L10" s="35" t="s">
+        <v>83</v>
+      </c>
       <c r="M10" s="35"/>
       <c r="N10" s="35"/>
       <c r="O10" s="35"/>
       <c r="P10" s="35"/>
       <c r="Q10" s="36"/>
-      <c r="R10" s="32" t="s">
-        <v>78</v>
+      <c r="R10" s="76">
+        <f t="shared" si="0"/>
+        <v>5</v>
       </c>
       <c r="S10" s="33" t="s">
         <v>71</v>
@@ -2244,11 +2592,18 @@
       <c r="U10" s="35">
         <v>7</v>
       </c>
-      <c r="V10" s="35"/>
-      <c r="W10" s="35"/>
-      <c r="X10" s="35"/>
-      <c r="Y10" s="35"/>
-      <c r="Z10" s="35"/>
+      <c r="V10" s="80">
+        <f>9.3/12</f>
+        <v>0.77500000000000002</v>
+      </c>
+      <c r="W10" s="84"/>
+      <c r="X10" s="80">
+        <v>0.75</v>
+      </c>
+      <c r="Y10" s="84"/>
+      <c r="Z10" s="80" t="s">
+        <v>85</v>
+      </c>
       <c r="AA10" s="35"/>
       <c r="AB10" s="35"/>
       <c r="AC10" s="35"/>
@@ -2259,8 +2614,8 @@
       <c r="AH10" s="59"/>
       <c r="AI10" s="59"/>
       <c r="AJ10" s="59"/>
-      <c r="AK10" s="59"/>
-      <c r="AL10" s="59"/>
+      <c r="AK10" s="92"/>
+      <c r="AL10" s="93"/>
       <c r="AM10" s="59"/>
       <c r="AN10" s="59"/>
       <c r="AO10" s="59"/>
@@ -2338,7 +2693,9 @@
       <c r="C11" s="31" t="s">
         <v>29</v>
       </c>
-      <c r="F11" s="63"/>
+      <c r="F11" s="63" t="s">
+        <v>75</v>
+      </c>
       <c r="G11" s="35" t="s">
         <v>75</v>
       </c>
@@ -2350,12 +2707,20 @@
         <v>75</v>
       </c>
       <c r="K11" s="35"/>
-      <c r="L11" s="35"/>
-      <c r="M11" s="35"/>
+      <c r="L11" s="35" t="s">
+        <v>83</v>
+      </c>
+      <c r="M11" s="35" t="s">
+        <v>74</v>
+      </c>
       <c r="N11" s="35"/>
       <c r="O11" s="35"/>
       <c r="P11" s="35"/>
       <c r="Q11" s="36"/>
+      <c r="R11" s="76">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
       <c r="S11" s="33"/>
       <c r="T11" s="34" t="s">
         <v>1</v>
@@ -2363,11 +2728,20 @@
       <c r="U11" s="35">
         <v>11</v>
       </c>
-      <c r="V11" s="35"/>
-      <c r="W11" s="35"/>
-      <c r="X11" s="35"/>
-      <c r="Y11" s="35"/>
-      <c r="Z11" s="35"/>
+      <c r="V11" s="80">
+        <f>(11+2/3)/12</f>
+        <v>0.97222222222222221</v>
+      </c>
+      <c r="W11" s="84"/>
+      <c r="X11" s="80">
+        <f>7.5/8</f>
+        <v>0.9375</v>
+      </c>
+      <c r="Y11" s="84"/>
+      <c r="Z11" s="80">
+        <f>16.75/19</f>
+        <v>0.88157894736842102</v>
+      </c>
       <c r="AA11" s="35"/>
       <c r="AB11" s="35"/>
       <c r="AC11" s="35"/>
@@ -2378,8 +2752,8 @@
       <c r="AH11" s="59"/>
       <c r="AI11" s="59"/>
       <c r="AJ11" s="59"/>
-      <c r="AK11" s="59"/>
-      <c r="AL11" s="59"/>
+      <c r="AK11" s="92"/>
+      <c r="AL11" s="95"/>
       <c r="AM11" s="59"/>
       <c r="AN11" s="59"/>
       <c r="AO11" s="59"/>
@@ -2457,7 +2831,9 @@
       <c r="C12" s="31" t="s">
         <v>31</v>
       </c>
-      <c r="F12" s="63"/>
+      <c r="F12" s="63" t="s">
+        <v>74</v>
+      </c>
       <c r="G12" s="35" t="s">
         <v>74</v>
       </c>
@@ -2470,15 +2846,22 @@
       <c r="J12" s="35" t="s">
         <v>74</v>
       </c>
-      <c r="K12" s="35"/>
-      <c r="L12" s="35"/>
-      <c r="M12" s="35"/>
+      <c r="K12" s="35" t="s">
+        <v>74</v>
+      </c>
+      <c r="L12" s="35" t="s">
+        <v>83</v>
+      </c>
+      <c r="M12" s="35" t="s">
+        <v>74</v>
+      </c>
       <c r="N12" s="35"/>
       <c r="O12" s="35"/>
       <c r="P12" s="35"/>
       <c r="Q12" s="36"/>
-      <c r="R12" s="32" t="s">
-        <v>78</v>
+      <c r="R12" s="76">
+        <f t="shared" si="0"/>
+        <v>7</v>
       </c>
       <c r="S12" s="33" t="s">
         <v>71</v>
@@ -2489,11 +2872,18 @@
       <c r="U12" s="35">
         <v>12</v>
       </c>
-      <c r="V12" s="35"/>
-      <c r="W12" s="35"/>
-      <c r="X12" s="35"/>
-      <c r="Y12" s="35"/>
-      <c r="Z12" s="35"/>
+      <c r="V12" s="80">
+        <v>1</v>
+      </c>
+      <c r="W12" s="84"/>
+      <c r="X12" s="80">
+        <v>0.875</v>
+      </c>
+      <c r="Y12" s="84"/>
+      <c r="Z12" s="80">
+        <f>16.5/19</f>
+        <v>0.86842105263157898</v>
+      </c>
       <c r="AA12" s="35"/>
       <c r="AB12" s="35"/>
       <c r="AC12" s="35"/>
@@ -2504,8 +2894,8 @@
       <c r="AH12" s="59"/>
       <c r="AI12" s="59"/>
       <c r="AJ12" s="59"/>
-      <c r="AK12" s="59"/>
-      <c r="AL12" s="59"/>
+      <c r="AK12" s="94"/>
+      <c r="AL12" s="96"/>
       <c r="AM12" s="59"/>
       <c r="AN12" s="59"/>
       <c r="AO12" s="59"/>
@@ -2583,7 +2973,9 @@
       <c r="C13" s="31" t="s">
         <v>33</v>
       </c>
-      <c r="F13" s="63"/>
+      <c r="F13" s="63" t="s">
+        <v>74</v>
+      </c>
       <c r="G13" s="35" t="s">
         <v>74</v>
       </c>
@@ -2596,15 +2988,22 @@
       <c r="J13" s="35" t="s">
         <v>74</v>
       </c>
-      <c r="K13" s="35"/>
-      <c r="L13" s="35"/>
-      <c r="M13" s="35"/>
+      <c r="K13" s="35" t="s">
+        <v>74</v>
+      </c>
+      <c r="L13" s="35" t="s">
+        <v>83</v>
+      </c>
+      <c r="M13" s="35" t="s">
+        <v>74</v>
+      </c>
       <c r="N13" s="35"/>
       <c r="O13" s="35"/>
       <c r="P13" s="35"/>
       <c r="Q13" s="36"/>
-      <c r="R13" s="32" t="s">
-        <v>78</v>
+      <c r="R13" s="76">
+        <f t="shared" si="0"/>
+        <v>7</v>
       </c>
       <c r="S13" s="33"/>
       <c r="T13" s="34" t="s">
@@ -2613,11 +3012,19 @@
       <c r="U13" s="35">
         <v>11</v>
       </c>
-      <c r="V13" s="35"/>
-      <c r="W13" s="35"/>
-      <c r="X13" s="35"/>
-      <c r="Y13" s="35"/>
-      <c r="Z13" s="35"/>
+      <c r="V13" s="80">
+        <v>1</v>
+      </c>
+      <c r="W13" s="84"/>
+      <c r="X13" s="80">
+        <f>7.5/8</f>
+        <v>0.9375</v>
+      </c>
+      <c r="Y13" s="84"/>
+      <c r="Z13" s="80">
+        <f>17.75/18</f>
+        <v>0.98611111111111116</v>
+      </c>
       <c r="AA13" s="35"/>
       <c r="AB13" s="35"/>
       <c r="AC13" s="35"/>
@@ -2707,7 +3114,9 @@
       <c r="C14" s="31" t="s">
         <v>37</v>
       </c>
-      <c r="F14" s="63"/>
+      <c r="F14" s="63" t="s">
+        <v>74</v>
+      </c>
       <c r="G14" s="35" t="s">
         <v>74</v>
       </c>
@@ -2720,15 +3129,22 @@
       <c r="J14" s="35" t="s">
         <v>74</v>
       </c>
-      <c r="K14" s="35"/>
-      <c r="L14" s="35"/>
-      <c r="M14" s="35"/>
+      <c r="K14" s="35" t="s">
+        <v>74</v>
+      </c>
+      <c r="L14" s="35" t="s">
+        <v>83</v>
+      </c>
+      <c r="M14" s="35" t="s">
+        <v>74</v>
+      </c>
       <c r="N14" s="35"/>
       <c r="O14" s="35"/>
       <c r="P14" s="35"/>
       <c r="Q14" s="36"/>
-      <c r="R14" s="32" t="s">
-        <v>78</v>
+      <c r="R14" s="76">
+        <f t="shared" si="0"/>
+        <v>7</v>
       </c>
       <c r="S14" s="33" t="s">
         <v>71</v>
@@ -2739,11 +3155,18 @@
       <c r="U14" s="35">
         <v>10</v>
       </c>
-      <c r="V14" s="35"/>
-      <c r="W14" s="35"/>
-      <c r="X14" s="35"/>
-      <c r="Y14" s="35"/>
-      <c r="Z14" s="35"/>
+      <c r="V14" s="80">
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="W14" s="84"/>
+      <c r="X14" s="80">
+        <v>0.875</v>
+      </c>
+      <c r="Y14" s="84"/>
+      <c r="Z14" s="80">
+        <f>18.25/19</f>
+        <v>0.96052631578947367</v>
+      </c>
       <c r="AA14" s="35"/>
       <c r="AB14" s="35"/>
       <c r="AC14" s="35"/>
@@ -2823,7 +3246,7 @@
       <c r="CY14" s="59"/>
       <c r="CZ14" s="59"/>
     </row>
-    <row r="15" spans="1:104" s="43" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:104" s="43" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A15" s="40" t="s">
         <v>38</v>
       </c>
@@ -2833,7 +3256,9 @@
       <c r="C15" s="42" t="s">
         <v>39</v>
       </c>
-      <c r="F15" s="64"/>
+      <c r="F15" s="64" t="s">
+        <v>75</v>
+      </c>
       <c r="G15" s="46" t="s">
         <v>75</v>
       </c>
@@ -2844,13 +3269,23 @@
       <c r="J15" s="46" t="s">
         <v>75</v>
       </c>
-      <c r="K15" s="46"/>
-      <c r="L15" s="46"/>
-      <c r="M15" s="46"/>
+      <c r="K15" s="46" t="s">
+        <v>75</v>
+      </c>
+      <c r="L15" s="46" t="s">
+        <v>83</v>
+      </c>
+      <c r="M15" s="46" t="s">
+        <v>75</v>
+      </c>
       <c r="N15" s="46"/>
       <c r="O15" s="46"/>
       <c r="P15" s="46"/>
       <c r="Q15" s="47"/>
+      <c r="R15" s="77">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
       <c r="S15" s="44" t="s">
         <v>71</v>
       </c>
@@ -2860,11 +3295,19 @@
       <c r="U15" s="46">
         <v>12</v>
       </c>
-      <c r="V15" s="46"/>
-      <c r="W15" s="46"/>
-      <c r="X15" s="46"/>
-      <c r="Y15" s="46"/>
-      <c r="Z15" s="46"/>
+      <c r="V15" s="81">
+        <v>1</v>
+      </c>
+      <c r="W15" s="85"/>
+      <c r="X15" s="81">
+        <f>7.5/8</f>
+        <v>0.9375</v>
+      </c>
+      <c r="Y15" s="85"/>
+      <c r="Z15" s="98">
+        <f>17.75/18</f>
+        <v>0.98611111111111116</v>
+      </c>
       <c r="AA15" s="46"/>
       <c r="AB15" s="46"/>
       <c r="AC15" s="46"/>
@@ -2944,7 +3387,7 @@
       <c r="CY15" s="60"/>
       <c r="CZ15" s="60"/>
     </row>
-    <row r="16" spans="1:104" s="32" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:104" s="32" customFormat="1" ht="15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A16" s="29" t="s">
         <v>42</v>
       </c>
@@ -2954,7 +3397,9 @@
       <c r="C16" s="31" t="s">
         <v>43</v>
       </c>
-      <c r="F16" s="63"/>
+      <c r="F16" s="63" t="s">
+        <v>74</v>
+      </c>
       <c r="G16" s="35" t="s">
         <v>74</v>
       </c>
@@ -2964,14 +3409,19 @@
       <c r="I16" s="35"/>
       <c r="J16" s="35"/>
       <c r="K16" s="35"/>
-      <c r="L16" s="35"/>
-      <c r="M16" s="35"/>
+      <c r="L16" s="35" t="s">
+        <v>83</v>
+      </c>
+      <c r="M16" s="35" t="s">
+        <v>74</v>
+      </c>
       <c r="N16" s="35"/>
       <c r="O16" s="35"/>
       <c r="P16" s="35"/>
       <c r="Q16" s="36"/>
-      <c r="R16" s="32" t="s">
-        <v>78</v>
+      <c r="R16" s="76">
+        <f t="shared" si="0"/>
+        <v>4</v>
       </c>
       <c r="S16" s="33" t="s">
         <v>71</v>
@@ -2982,12 +3432,20 @@
       <c r="U16" s="35">
         <v>0</v>
       </c>
-      <c r="V16" s="35"/>
-      <c r="W16" s="35"/>
-      <c r="X16" s="35"/>
-      <c r="Y16" s="35"/>
-      <c r="Z16" s="35"/>
-      <c r="AA16" s="35"/>
+      <c r="V16" s="80">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="W16" s="84"/>
+      <c r="X16" s="88">
+        <f>4.5/8</f>
+        <v>0.5625</v>
+      </c>
+      <c r="Y16" s="87"/>
+      <c r="Z16" s="97">
+        <f>7.25/18</f>
+        <v>0.40277777777777779</v>
+      </c>
+      <c r="AA16" s="34"/>
       <c r="AB16" s="35"/>
       <c r="AC16" s="35"/>
       <c r="AD16" s="35"/>
@@ -3066,7 +3524,7 @@
       <c r="CY16" s="59"/>
       <c r="CZ16" s="59"/>
     </row>
-    <row r="17" spans="1:104" s="32" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:104" s="32" customFormat="1" ht="15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A17" s="29" t="s">
         <v>48</v>
       </c>
@@ -3076,7 +3534,9 @@
       <c r="C17" s="31" t="s">
         <v>49</v>
       </c>
-      <c r="F17" s="63"/>
+      <c r="F17" s="63" t="s">
+        <v>74</v>
+      </c>
       <c r="G17" s="35" t="s">
         <v>74</v>
       </c>
@@ -3086,12 +3546,18 @@
       <c r="I17" s="35"/>
       <c r="J17" s="35"/>
       <c r="K17" s="35"/>
-      <c r="L17" s="35"/>
+      <c r="L17" s="35" t="s">
+        <v>83</v>
+      </c>
       <c r="M17" s="35"/>
       <c r="N17" s="35"/>
       <c r="O17" s="35"/>
       <c r="P17" s="35"/>
       <c r="Q17" s="36"/>
+      <c r="R17" s="76">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
       <c r="S17" s="33"/>
       <c r="T17" s="34" t="s">
         <v>1</v>
@@ -3099,12 +3565,20 @@
       <c r="U17" s="35">
         <v>1</v>
       </c>
-      <c r="V17" s="35"/>
-      <c r="W17" s="35"/>
-      <c r="X17" s="35"/>
-      <c r="Y17" s="35"/>
-      <c r="Z17" s="35"/>
-      <c r="AA17" s="35"/>
+      <c r="V17" s="80">
+        <v>0.125</v>
+      </c>
+      <c r="W17" s="87"/>
+      <c r="X17" s="97">
+        <f>2.5/8</f>
+        <v>0.3125</v>
+      </c>
+      <c r="Y17" s="99"/>
+      <c r="Z17" s="97">
+        <f>6.5/18</f>
+        <v>0.3611111111111111</v>
+      </c>
+      <c r="AA17" s="34"/>
       <c r="AB17" s="35"/>
       <c r="AC17" s="35"/>
       <c r="AD17" s="35"/>
@@ -3183,7 +3657,7 @@
       <c r="CY17" s="59"/>
       <c r="CZ17" s="59"/>
     </row>
-    <row r="18" spans="1:104" s="32" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:104" s="32" customFormat="1" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A18" s="29" t="s">
         <v>52</v>
       </c>
@@ -3193,7 +3667,9 @@
       <c r="C18" s="31" t="s">
         <v>53</v>
       </c>
-      <c r="F18" s="63"/>
+      <c r="F18" s="63" t="s">
+        <v>74</v>
+      </c>
       <c r="G18" s="35" t="s">
         <v>74</v>
       </c>
@@ -3206,15 +3682,22 @@
       <c r="J18" s="35" t="s">
         <v>74</v>
       </c>
-      <c r="K18" s="35"/>
-      <c r="L18" s="35"/>
-      <c r="M18" s="35"/>
+      <c r="K18" s="35" t="s">
+        <v>74</v>
+      </c>
+      <c r="L18" s="35" t="s">
+        <v>83</v>
+      </c>
+      <c r="M18" s="35" t="s">
+        <v>74</v>
+      </c>
       <c r="N18" s="35"/>
       <c r="O18" s="35"/>
       <c r="P18" s="35"/>
       <c r="Q18" s="36"/>
-      <c r="R18" s="32" t="s">
-        <v>78</v>
+      <c r="R18" s="76">
+        <f t="shared" si="0"/>
+        <v>7</v>
       </c>
       <c r="S18" s="33" t="s">
         <v>71</v>
@@ -3225,11 +3708,18 @@
       <c r="U18" s="35">
         <v>12</v>
       </c>
-      <c r="V18" s="35"/>
-      <c r="W18" s="35"/>
-      <c r="X18" s="35"/>
-      <c r="Y18" s="35"/>
-      <c r="Z18" s="35"/>
+      <c r="V18" s="80">
+        <v>1</v>
+      </c>
+      <c r="W18" s="84"/>
+      <c r="X18" s="89">
+        <v>1</v>
+      </c>
+      <c r="Y18" s="84"/>
+      <c r="Z18" s="89">
+        <f>17.75/18</f>
+        <v>0.98611111111111116</v>
+      </c>
       <c r="AA18" s="35"/>
       <c r="AB18" s="35"/>
       <c r="AC18" s="35"/>
@@ -3319,7 +3809,9 @@
       <c r="C19" s="42" t="s">
         <v>61</v>
       </c>
-      <c r="F19" s="64"/>
+      <c r="F19" s="64" t="s">
+        <v>74</v>
+      </c>
       <c r="G19" s="46" t="s">
         <v>74</v>
       </c>
@@ -3332,13 +3824,23 @@
       <c r="J19" s="46" t="s">
         <v>74</v>
       </c>
-      <c r="K19" s="46"/>
-      <c r="L19" s="46"/>
-      <c r="M19" s="46"/>
+      <c r="K19" s="46" t="s">
+        <v>74</v>
+      </c>
+      <c r="L19" s="46" t="s">
+        <v>83</v>
+      </c>
+      <c r="M19" s="46" t="s">
+        <v>74</v>
+      </c>
       <c r="N19" s="46"/>
       <c r="O19" s="46"/>
       <c r="P19" s="46"/>
       <c r="Q19" s="47"/>
+      <c r="R19" s="77">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
       <c r="S19" s="44" t="s">
         <v>0</v>
       </c>
@@ -3348,11 +3850,18 @@
       <c r="U19" s="46">
         <v>11</v>
       </c>
-      <c r="V19" s="46"/>
-      <c r="W19" s="46"/>
-      <c r="X19" s="46"/>
-      <c r="Y19" s="46"/>
-      <c r="Z19" s="46"/>
+      <c r="V19" s="81">
+        <v>1</v>
+      </c>
+      <c r="W19" s="85"/>
+      <c r="X19" s="81">
+        <v>0.625</v>
+      </c>
+      <c r="Y19" s="85"/>
+      <c r="Z19" s="81">
+        <f>15.5/18</f>
+        <v>0.86111111111111116</v>
+      </c>
       <c r="AA19" s="46"/>
       <c r="AB19" s="46"/>
       <c r="AC19" s="46"/>
@@ -3442,7 +3951,9 @@
       <c r="C20" s="39" t="s">
         <v>63</v>
       </c>
-      <c r="F20" s="65"/>
+      <c r="F20" s="65" t="s">
+        <v>74</v>
+      </c>
       <c r="G20" s="56" t="s">
         <v>74</v>
       </c>
@@ -3455,15 +3966,22 @@
       <c r="J20" s="56" t="s">
         <v>74</v>
       </c>
-      <c r="K20" s="56"/>
-      <c r="L20" s="56"/>
-      <c r="M20" s="56"/>
+      <c r="K20" s="56" t="s">
+        <v>75</v>
+      </c>
+      <c r="L20" s="56" t="s">
+        <v>83</v>
+      </c>
+      <c r="M20" s="56" t="s">
+        <v>75</v>
+      </c>
       <c r="N20" s="56"/>
       <c r="O20" s="56"/>
       <c r="P20" s="56"/>
       <c r="Q20" s="57"/>
-      <c r="R20" s="32" t="s">
-        <v>78</v>
+      <c r="R20" s="76">
+        <f t="shared" si="0"/>
+        <v>7</v>
       </c>
       <c r="S20" s="54"/>
       <c r="T20" s="55" t="s">
@@ -3472,11 +3990,18 @@
       <c r="U20" s="56">
         <v>6</v>
       </c>
-      <c r="V20" s="56"/>
-      <c r="W20" s="56"/>
-      <c r="X20" s="56"/>
-      <c r="Y20" s="56"/>
-      <c r="Z20" s="56"/>
+      <c r="V20" s="82">
+        <v>0.75</v>
+      </c>
+      <c r="W20" s="86"/>
+      <c r="X20" s="82">
+        <v>0.875</v>
+      </c>
+      <c r="Y20" s="86"/>
+      <c r="Z20" s="82">
+        <f>14/19</f>
+        <v>0.73684210526315785</v>
+      </c>
       <c r="AA20" s="56"/>
       <c r="AB20" s="56"/>
       <c r="AC20" s="56"/>
@@ -3561,19 +4086,19 @@
       <c r="B21" s="72"/>
       <c r="C21" s="71"/>
       <c r="F21" s="72">
-        <f t="shared" ref="F21:I21" si="0">COUNTA(F4:F20)</f>
-        <v>0</v>
+        <f t="shared" ref="F21:I21" si="1">COUNTA(F4:F20)</f>
+        <v>17</v>
       </c>
       <c r="G21" s="72">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>17</v>
       </c>
       <c r="H21" s="72">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>13</v>
       </c>
       <c r="I21" s="72">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>15</v>
       </c>
       <c r="J21" s="72">
@@ -3581,47 +4106,58 @@
         <v>13</v>
       </c>
       <c r="K21" s="72">
-        <f t="shared" ref="K21:Q21" si="1">COUNTA(K4:K20)</f>
+        <f t="shared" ref="K21:Q21" si="2">COUNTA(K4:K20)</f>
+        <v>11</v>
+      </c>
+      <c r="L21" s="72">
+        <f t="shared" si="2"/>
+        <v>17</v>
+      </c>
+      <c r="M21" s="72">
+        <f t="shared" si="2"/>
+        <v>12</v>
+      </c>
+      <c r="N21" s="72">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="L21" s="72">
-        <f t="shared" si="1"/>
+      <c r="O21" s="72">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="M21" s="72">
-        <f t="shared" si="1"/>
+      <c r="P21" s="72">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="N21" s="72">
-        <f t="shared" si="1"/>
+      <c r="Q21" s="72">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="O21" s="72">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="P21" s="72">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="Q21" s="72">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
+      <c r="R21" s="78"/>
       <c r="S21" s="72"/>
       <c r="T21" s="72"/>
       <c r="U21" s="72"/>
-      <c r="V21" s="72"/>
+      <c r="V21" s="100">
+        <v>0.1</v>
+      </c>
       <c r="W21" s="72"/>
-      <c r="X21" s="72"/>
+      <c r="X21" s="100">
+        <v>0.15</v>
+      </c>
       <c r="Y21" s="72"/>
-      <c r="Z21" s="72"/>
+      <c r="Z21" s="100">
+        <v>0.15</v>
+      </c>
       <c r="AA21" s="72"/>
       <c r="AB21" s="72"/>
-      <c r="AC21" s="72"/>
+      <c r="AC21" s="100">
+        <v>0.1</v>
+      </c>
       <c r="AD21" s="72"/>
       <c r="AE21" s="72"/>
-      <c r="AF21" s="72"/>
+      <c r="AF21" s="100">
+        <v>0.4</v>
+      </c>
     </row>
     <row r="22" spans="1:104" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="71"/>
@@ -3639,6 +4175,7 @@
       <c r="O22" s="72"/>
       <c r="P22" s="72"/>
       <c r="Q22" s="72"/>
+      <c r="R22" s="78"/>
       <c r="S22" s="72"/>
       <c r="T22" s="72"/>
       <c r="U22" s="72"/>
@@ -3670,6 +4207,7 @@
       <c r="O23" s="72"/>
       <c r="P23" s="72"/>
       <c r="Q23" s="72"/>
+      <c r="R23" s="78"/>
       <c r="S23" s="72"/>
       <c r="T23" s="72"/>
       <c r="U23" s="72"/>
@@ -3699,6 +4237,7 @@
       <c r="O24" s="19"/>
       <c r="P24" s="19"/>
       <c r="Q24" s="19"/>
+      <c r="R24" s="79"/>
       <c r="S24" s="19"/>
       <c r="T24" s="19"/>
       <c r="U24" s="19"/>
@@ -3981,7 +4520,9 @@
       <c r="J29" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="K29" s="7"/>
+      <c r="K29" s="7" t="s">
+        <v>74</v>
+      </c>
       <c r="L29" s="7"/>
       <c r="M29" s="7"/>
       <c r="N29" s="7"/>
@@ -4426,6 +4967,7 @@
       <c r="O41" s="35"/>
       <c r="P41" s="35"/>
       <c r="Q41" s="36"/>
+      <c r="R41" s="76"/>
       <c r="S41" s="33"/>
       <c r="T41" s="34"/>
       <c r="U41" s="35"/>
@@ -4520,8 +5062,11 @@
     <hyperlink ref="C6" r:id="rId3" xr:uid="{1D032707-CB5E-47EB-BEE8-B7BEC4DD4851}"/>
     <hyperlink ref="C16" r:id="rId4" xr:uid="{86F6773C-8983-492A-B4ED-8DF22E016661}"/>
   </hyperlinks>
-  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" fitToHeight="0" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId5"/>
+  <colBreaks count="1" manualBreakCount="1">
+    <brk id="17" max="1048575" man="1"/>
+  </colBreaks>
   <drawing r:id="rId6"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Course delivered. Everything needs tidying up but everything presented is here.
</commit_message>
<xml_diff>
--- a/admin/LIN6209 student data.xlsx
+++ b/admin/LIN6209 student data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/138e04b35f3df159/AllTeaching/_QMUL/LIN6209/admin/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="655" documentId="8_{D4084AF5-A7E0-4A89-8908-66192E3C3F85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ED532B37-0EDE-4144-A464-E414EC704DCA}"/>
+  <xr:revisionPtr revIDLastSave="790" documentId="8_{D4084AF5-A7E0-4A89-8908-66192E3C3F85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B5786537-6537-4D00-9406-AFE7F958FC1C}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21820" xr2:uid="{FBA493EA-9E30-4955-99CC-D2245AEE8977}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="101">
   <si>
     <t>F</t>
   </si>
@@ -278,9 +278,6 @@
     <t>Lin6209 Coding for Linguists</t>
   </si>
   <si>
-    <t>I</t>
-  </si>
-  <si>
     <t>Attendance</t>
   </si>
   <si>
@@ -296,10 +293,55 @@
     <t>*</t>
   </si>
   <si>
-    <t>*24th</t>
-  </si>
-  <si>
     <t>**</t>
+  </si>
+  <si>
+    <t>Coding for Linguists</t>
+  </si>
+  <si>
+    <t>Assessment:</t>
+  </si>
+  <si>
+    <t>Item 1: 20% 4 Quizzes (5 SAQ x 4)</t>
+  </si>
+  <si>
+    <t>Item 2: 30% Portfolio of Lab Work (Equivalent to 1000 words)</t>
+  </si>
+  <si>
+    <t>Item 3: 50% Assignment (Equivalent to 2000 words)</t>
+  </si>
+  <si>
+    <t>Credits: 15.0</t>
+  </si>
+  <si>
+    <t>Contact: Mr Peter Mcginty</t>
+  </si>
+  <si>
+    <t>Overlap: None</t>
+  </si>
+  <si>
+    <t>Prerequisite: None</t>
+  </si>
+  <si>
+    <t>Corequisite: None</t>
+  </si>
+  <si>
+    <t>Description: This module provides students with an introduction to computer programming and computational modelling for applied linguistics. Students will learn how to write code in a widely used programming language (Python), and gain experience in using tools that are suited to solving a range of computational problems in linguistics using machine learning approaches. There will be a focus on developing practical skills. The module is suitable for final year BA students and MA students without any prior experience in computer programming or machine learning.</t>
+  </si>
+  <si>
+    <t>Level: 6</t>
+  </si>
+  <si>
+    <t>Weighting</t>
+  </si>
+  <si>
+    <t>Av score</t>
+  </si>
+  <si>
+    <t>Total Marks</t>
+  </si>
+  <si>
+    <t>=[[w2a]]*0.10+ [[w4]]*0.15 + [[w6]]*0.20 + [[pp1]]*0.10 + [[pp2]]*0.45 + [[contrib]]*0.0</t>
   </si>
 </sst>
 </file>
@@ -309,7 +351,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -354,6 +396,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -373,7 +423,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="41">
+  <borders count="34">
     <border>
       <left/>
       <right/>
@@ -789,83 +839,6 @@
       <top/>
       <bottom style="thin">
         <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFFF0000"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color rgb="FFFF0000"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color rgb="FFFF0000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFFF0000"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFFF0000"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color rgb="FFFF0000"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFFF0000"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color rgb="FFFF0000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFFF0000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFFF0000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFFF0000"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFFF0000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFFF0000"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color rgb="FFFF0000"/>
       </bottom>
       <diagonal/>
     </border>
@@ -903,7 +876,7 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="101">
+  <cellXfs count="99">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1122,25 +1095,25 @@
     <xf numFmtId="9" fontId="3" fillId="2" borderId="31" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="32" xfId="2" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="33" xfId="2" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="34" xfId="2" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="35" xfId="2" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="36" xfId="2" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="37" xfId="2" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="38" xfId="2" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="3" fillId="2" borderId="39" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="3" fillId="2" borderId="32" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="9" fontId="4" fillId="3" borderId="30" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="3" fillId="2" borderId="40" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="3" fillId="2" borderId="33" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="3" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" xfId="4" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Good" xfId="2" builtinId="26"/>
@@ -1149,7 +1122,18 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="4" builtinId="5"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1562,7 +1546,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="Z5" sqref="Z5"/>
+      <selection pane="topRight" activeCell="AG18" sqref="AG18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1580,11 +1564,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:104" x14ac:dyDescent="0.35">
-      <c r="F1" t="s">
+      <c r="F1" s="96" t="s">
+        <v>79</v>
+      </c>
+      <c r="T1" s="96" t="s">
         <v>80</v>
-      </c>
-      <c r="T1" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="2" spans="1:104" ht="21.5" thickBot="1" x14ac:dyDescent="0.55000000000000004">
@@ -1601,7 +1585,7 @@
         <v>44480</v>
       </c>
       <c r="I2" s="73" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J2" s="73">
         <v>44494</v>
@@ -1717,6 +1701,9 @@
       <c r="AF3" s="4">
         <v>12</v>
       </c>
+      <c r="AG3" s="58" t="s">
+        <v>99</v>
+      </c>
     </row>
     <row r="4" spans="1:104" s="32" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="29" t="s">
@@ -1747,18 +1734,22 @@
         <v>74</v>
       </c>
       <c r="L4" s="74" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="M4" s="35" t="s">
         <v>74</v>
       </c>
-      <c r="N4" s="35"/>
-      <c r="O4" s="35"/>
+      <c r="N4" s="35" t="s">
+        <v>74</v>
+      </c>
+      <c r="O4" s="35" t="s">
+        <v>74</v>
+      </c>
       <c r="P4" s="35"/>
       <c r="Q4" s="36"/>
       <c r="R4" s="76">
         <f>COUNTIFS(F4:Q4, "P")+COUNTIFS(F4:Q4, "O")</f>
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="S4" s="33" t="s">
         <v>0</v>
@@ -1783,14 +1774,22 @@
         <v>0.73611111111111116</v>
       </c>
       <c r="AA4" s="35"/>
-      <c r="AB4" s="35"/>
+      <c r="AB4" s="80">
+        <f>7/10</f>
+        <v>0.7</v>
+      </c>
       <c r="AC4" s="35"/>
       <c r="AD4" s="35"/>
       <c r="AE4" s="35"/>
       <c r="AF4" s="36"/>
-      <c r="AG4" s="59"/>
+      <c r="AG4" s="97">
+        <f>V4*0.1+X4*0.15+Z4*0.2+AB4*0.1+AF4*0.45</f>
+        <v>0.39795138888888887</v>
+      </c>
       <c r="AH4" s="59"/>
-      <c r="AI4" s="59"/>
+      <c r="AI4" s="98" t="s">
+        <v>100</v>
+      </c>
       <c r="AJ4" s="59"/>
       <c r="AK4" s="59"/>
       <c r="AL4" s="59"/>
@@ -1888,7 +1887,7 @@
       </c>
       <c r="K5" s="35"/>
       <c r="L5" s="74" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="M5" s="35"/>
       <c r="N5" s="35"/>
@@ -1911,20 +1910,26 @@
         <v>0.75</v>
       </c>
       <c r="W5" s="84"/>
-      <c r="X5" s="80" t="s">
-        <v>85</v>
+      <c r="X5" s="80">
+        <f>6/8</f>
+        <v>0.75</v>
       </c>
       <c r="Y5" s="84"/>
-      <c r="Z5" s="83" t="s">
-        <v>84</v>
-      </c>
-      <c r="AA5" s="35"/>
-      <c r="AB5" s="35"/>
+      <c r="Z5" s="83">
+        <v>0</v>
+      </c>
+      <c r="AA5" s="35" t="s">
+        <v>83</v>
+      </c>
+      <c r="AB5" s="80"/>
       <c r="AC5" s="35"/>
       <c r="AD5" s="35"/>
       <c r="AE5" s="35"/>
       <c r="AF5" s="36"/>
-      <c r="AG5" s="59"/>
+      <c r="AG5" s="97">
+        <f t="shared" ref="AG5:AG20" si="1">V5*0.1+X5*0.15+Z5*0.2+AB5*0.1+AF5*0.45</f>
+        <v>0.1875</v>
+      </c>
       <c r="AH5" s="59"/>
       <c r="AI5" s="59"/>
       <c r="AJ5" s="59"/>
@@ -2026,18 +2031,24 @@
         <v>74</v>
       </c>
       <c r="L6" s="35" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="M6" s="35" t="s">
         <v>75</v>
       </c>
-      <c r="N6" s="35"/>
-      <c r="O6" s="35"/>
-      <c r="P6" s="35"/>
+      <c r="N6" s="35" t="s">
+        <v>74</v>
+      </c>
+      <c r="O6" s="35" t="s">
+        <v>74</v>
+      </c>
+      <c r="P6" s="35" t="s">
+        <v>75</v>
+      </c>
       <c r="Q6" s="36"/>
       <c r="R6" s="76">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="S6" s="33"/>
       <c r="T6" s="34" t="s">
@@ -2059,12 +2070,18 @@
         <v>0.86111111111111116</v>
       </c>
       <c r="AA6" s="35"/>
-      <c r="AB6" s="35"/>
+      <c r="AB6" s="80">
+        <f>5/10</f>
+        <v>0.5</v>
+      </c>
       <c r="AC6" s="35"/>
       <c r="AD6" s="35"/>
       <c r="AE6" s="35"/>
       <c r="AF6" s="36"/>
-      <c r="AG6" s="59"/>
+      <c r="AG6" s="97">
+        <f t="shared" si="1"/>
+        <v>0.38263888888888892</v>
+      </c>
       <c r="AH6" s="59"/>
       <c r="AI6" s="59"/>
       <c r="AJ6" s="59"/>
@@ -2157,21 +2174,25 @@
         <v>74</v>
       </c>
       <c r="I7" s="35" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="J7" s="35"/>
       <c r="K7" s="35"/>
       <c r="L7" s="35" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="M7" s="35"/>
-      <c r="N7" s="35"/>
+      <c r="N7" s="35" t="s">
+        <v>75</v>
+      </c>
       <c r="O7" s="35"/>
-      <c r="P7" s="35"/>
+      <c r="P7" s="35" t="s">
+        <v>75</v>
+      </c>
       <c r="Q7" s="36"/>
       <c r="R7" s="76">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="S7" s="33" t="s">
         <v>70</v>
@@ -2190,22 +2211,27 @@
         <v>0.9375</v>
       </c>
       <c r="Y7" s="84"/>
-      <c r="Z7" s="83" t="s">
-        <v>86</v>
-      </c>
-      <c r="AA7" s="35"/>
-      <c r="AB7" s="35"/>
+      <c r="Z7" s="83">
+        <v>0</v>
+      </c>
+      <c r="AA7" s="35" t="s">
+        <v>84</v>
+      </c>
+      <c r="AB7" s="80"/>
       <c r="AC7" s="35"/>
       <c r="AD7" s="35"/>
       <c r="AE7" s="35"/>
       <c r="AF7" s="36"/>
-      <c r="AG7" s="59"/>
+      <c r="AG7" s="97">
+        <f t="shared" si="1"/>
+        <v>0.22645833333333334</v>
+      </c>
       <c r="AH7" s="59"/>
       <c r="AI7" s="59"/>
-      <c r="AJ7" s="59"/>
-      <c r="AK7" s="59"/>
-      <c r="AL7" s="59"/>
-      <c r="AM7" s="59"/>
+      <c r="AJ7" s="71"/>
+      <c r="AK7" s="71"/>
+      <c r="AL7" s="71"/>
+      <c r="AM7" s="71"/>
       <c r="AN7" s="59"/>
       <c r="AO7" s="59"/>
       <c r="AP7" s="59"/>
@@ -2301,18 +2327,22 @@
         <v>74</v>
       </c>
       <c r="L8" s="35" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="M8" s="35" t="s">
         <v>74</v>
       </c>
-      <c r="N8" s="35"/>
-      <c r="O8" s="35"/>
+      <c r="N8" s="35" t="s">
+        <v>74</v>
+      </c>
+      <c r="O8" s="35" t="s">
+        <v>74</v>
+      </c>
       <c r="P8" s="35"/>
       <c r="Q8" s="36"/>
       <c r="R8" s="76">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="S8" s="33"/>
       <c r="T8" s="34" t="s">
@@ -2334,18 +2364,26 @@
         <v>0.81944444444444442</v>
       </c>
       <c r="AA8" s="35"/>
-      <c r="AB8" s="35"/>
+      <c r="AB8" s="80">
+        <f>9/10</f>
+        <v>0.9</v>
+      </c>
       <c r="AC8" s="35"/>
       <c r="AD8" s="35"/>
       <c r="AE8" s="35"/>
       <c r="AF8" s="36"/>
-      <c r="AG8" s="59"/>
+      <c r="AG8" s="97">
+        <f t="shared" si="1"/>
+        <v>0.48513888888888895</v>
+      </c>
       <c r="AH8" s="59"/>
-      <c r="AI8" s="59"/>
-      <c r="AJ8" s="59"/>
-      <c r="AK8" s="90"/>
-      <c r="AL8" s="91"/>
-      <c r="AM8" s="59"/>
+      <c r="AI8" s="59" t="s">
+        <v>85</v>
+      </c>
+      <c r="AJ8" s="71"/>
+      <c r="AK8" s="71"/>
+      <c r="AL8" s="71"/>
+      <c r="AM8" s="71"/>
       <c r="AN8" s="59"/>
       <c r="AO8" s="59"/>
       <c r="AP8" s="59"/>
@@ -2435,7 +2473,7 @@
       <c r="J9" s="35"/>
       <c r="K9" s="35"/>
       <c r="L9" s="35" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="M9" s="35"/>
       <c r="N9" s="35"/>
@@ -2467,18 +2505,26 @@
         <v>0.93421052631578949</v>
       </c>
       <c r="AA9" s="35"/>
-      <c r="AB9" s="35"/>
+      <c r="AB9" s="80">
+        <f>7/10</f>
+        <v>0.7</v>
+      </c>
       <c r="AC9" s="35"/>
       <c r="AD9" s="35"/>
       <c r="AE9" s="35"/>
       <c r="AF9" s="36"/>
-      <c r="AG9" s="59"/>
+      <c r="AG9" s="97">
+        <f t="shared" si="1"/>
+        <v>0.47975877192982458</v>
+      </c>
       <c r="AH9" s="59"/>
-      <c r="AI9" s="59"/>
-      <c r="AJ9" s="59"/>
-      <c r="AK9" s="92"/>
-      <c r="AL9" s="93"/>
-      <c r="AM9" s="59"/>
+      <c r="AI9" s="59" t="s">
+        <v>90</v>
+      </c>
+      <c r="AJ9" s="71"/>
+      <c r="AK9" s="71"/>
+      <c r="AL9" s="71"/>
+      <c r="AM9" s="71"/>
       <c r="AN9" s="59"/>
       <c r="AO9" s="59"/>
       <c r="AP9" s="59"/>
@@ -2572,16 +2618,22 @@
         <v>75</v>
       </c>
       <c r="L10" s="35" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="M10" s="35"/>
-      <c r="N10" s="35"/>
-      <c r="O10" s="35"/>
-      <c r="P10" s="35"/>
+      <c r="N10" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="O10" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="P10" s="35" t="s">
+        <v>75</v>
+      </c>
       <c r="Q10" s="36"/>
       <c r="R10" s="76">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="S10" s="33" t="s">
         <v>71</v>
@@ -2601,22 +2653,31 @@
         <v>0.75</v>
       </c>
       <c r="Y10" s="84"/>
-      <c r="Z10" s="80" t="s">
-        <v>85</v>
+      <c r="Z10" s="80">
+        <f>15.5/18</f>
+        <v>0.86111111111111116</v>
       </c>
       <c r="AA10" s="35"/>
-      <c r="AB10" s="35"/>
+      <c r="AB10" s="80">
+        <f>6/10</f>
+        <v>0.6</v>
+      </c>
       <c r="AC10" s="35"/>
       <c r="AD10" s="35"/>
       <c r="AE10" s="35"/>
       <c r="AF10" s="36"/>
-      <c r="AG10" s="59"/>
+      <c r="AG10" s="97">
+        <f t="shared" si="1"/>
+        <v>0.42222222222222222</v>
+      </c>
       <c r="AH10" s="59"/>
-      <c r="AI10" s="59"/>
-      <c r="AJ10" s="59"/>
-      <c r="AK10" s="92"/>
-      <c r="AL10" s="93"/>
-      <c r="AM10" s="59"/>
+      <c r="AI10" s="59" t="s">
+        <v>91</v>
+      </c>
+      <c r="AJ10" s="71"/>
+      <c r="AK10" s="71"/>
+      <c r="AL10" s="71"/>
+      <c r="AM10" s="71"/>
       <c r="AN10" s="59"/>
       <c r="AO10" s="59"/>
       <c r="AP10" s="59"/>
@@ -2708,18 +2769,22 @@
       </c>
       <c r="K11" s="35"/>
       <c r="L11" s="35" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="M11" s="35" t="s">
         <v>74</v>
       </c>
-      <c r="N11" s="35"/>
+      <c r="N11" s="35" t="s">
+        <v>75</v>
+      </c>
       <c r="O11" s="35"/>
-      <c r="P11" s="35"/>
+      <c r="P11" s="35" t="s">
+        <v>74</v>
+      </c>
       <c r="Q11" s="36"/>
       <c r="R11" s="76">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="S11" s="33"/>
       <c r="T11" s="34" t="s">
@@ -2743,18 +2808,26 @@
         <v>0.88157894736842102</v>
       </c>
       <c r="AA11" s="35"/>
-      <c r="AB11" s="35"/>
+      <c r="AB11" s="80">
+        <f>10/10</f>
+        <v>1</v>
+      </c>
       <c r="AC11" s="35"/>
       <c r="AD11" s="35"/>
       <c r="AE11" s="35"/>
       <c r="AF11" s="36"/>
-      <c r="AG11" s="59"/>
+      <c r="AG11" s="97">
+        <f t="shared" si="1"/>
+        <v>0.51416301169590639</v>
+      </c>
       <c r="AH11" s="59"/>
-      <c r="AI11" s="59"/>
-      <c r="AJ11" s="59"/>
-      <c r="AK11" s="92"/>
-      <c r="AL11" s="95"/>
-      <c r="AM11" s="59"/>
+      <c r="AI11" s="59" t="s">
+        <v>92</v>
+      </c>
+      <c r="AJ11" s="71"/>
+      <c r="AK11" s="71"/>
+      <c r="AL11" s="71"/>
+      <c r="AM11" s="71"/>
       <c r="AN11" s="59"/>
       <c r="AO11" s="59"/>
       <c r="AP11" s="59"/>
@@ -2850,18 +2923,24 @@
         <v>74</v>
       </c>
       <c r="L12" s="35" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="M12" s="35" t="s">
         <v>74</v>
       </c>
-      <c r="N12" s="35"/>
-      <c r="O12" s="35"/>
-      <c r="P12" s="35"/>
+      <c r="N12" s="35" t="s">
+        <v>74</v>
+      </c>
+      <c r="O12" s="35" t="s">
+        <v>74</v>
+      </c>
+      <c r="P12" s="35" t="s">
+        <v>75</v>
+      </c>
       <c r="Q12" s="36"/>
       <c r="R12" s="76">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="S12" s="33" t="s">
         <v>71</v>
@@ -2885,18 +2964,26 @@
         <v>0.86842105263157898</v>
       </c>
       <c r="AA12" s="35"/>
-      <c r="AB12" s="35"/>
+      <c r="AB12" s="80">
+        <f>7/10</f>
+        <v>0.7</v>
+      </c>
       <c r="AC12" s="35"/>
       <c r="AD12" s="35"/>
       <c r="AE12" s="35"/>
       <c r="AF12" s="36"/>
-      <c r="AG12" s="59"/>
+      <c r="AG12" s="97">
+        <f t="shared" si="1"/>
+        <v>0.47493421052631585</v>
+      </c>
       <c r="AH12" s="59"/>
-      <c r="AI12" s="59"/>
-      <c r="AJ12" s="59"/>
-      <c r="AK12" s="94"/>
-      <c r="AL12" s="96"/>
-      <c r="AM12" s="59"/>
+      <c r="AI12" s="59" t="s">
+        <v>93</v>
+      </c>
+      <c r="AJ12" s="71"/>
+      <c r="AK12" s="71"/>
+      <c r="AL12" s="71"/>
+      <c r="AM12" s="71"/>
       <c r="AN12" s="59"/>
       <c r="AO12" s="59"/>
       <c r="AP12" s="59"/>
@@ -2992,18 +3079,24 @@
         <v>74</v>
       </c>
       <c r="L13" s="35" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="M13" s="35" t="s">
         <v>74</v>
       </c>
-      <c r="N13" s="35"/>
-      <c r="O13" s="35"/>
-      <c r="P13" s="35"/>
+      <c r="N13" s="35" t="s">
+        <v>74</v>
+      </c>
+      <c r="O13" s="35" t="s">
+        <v>74</v>
+      </c>
+      <c r="P13" s="35" t="s">
+        <v>74</v>
+      </c>
       <c r="Q13" s="36"/>
       <c r="R13" s="76">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="S13" s="33"/>
       <c r="T13" s="34" t="s">
@@ -3026,18 +3119,26 @@
         <v>0.98611111111111116</v>
       </c>
       <c r="AA13" s="35"/>
-      <c r="AB13" s="35"/>
+      <c r="AB13" s="80">
+        <f>9/10</f>
+        <v>0.9</v>
+      </c>
       <c r="AC13" s="35"/>
       <c r="AD13" s="35"/>
       <c r="AE13" s="35"/>
       <c r="AF13" s="36"/>
-      <c r="AG13" s="59"/>
+      <c r="AG13" s="97">
+        <f t="shared" si="1"/>
+        <v>0.52784722222222225</v>
+      </c>
       <c r="AH13" s="59"/>
-      <c r="AI13" s="59"/>
-      <c r="AJ13" s="59"/>
-      <c r="AK13" s="59"/>
-      <c r="AL13" s="59"/>
-      <c r="AM13" s="59"/>
+      <c r="AI13" s="59" t="s">
+        <v>94</v>
+      </c>
+      <c r="AJ13" s="71"/>
+      <c r="AK13" s="71"/>
+      <c r="AL13" s="71"/>
+      <c r="AM13" s="71"/>
       <c r="AN13" s="59"/>
       <c r="AO13" s="59"/>
       <c r="AP13" s="59"/>
@@ -3133,18 +3234,24 @@
         <v>74</v>
       </c>
       <c r="L14" s="35" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="M14" s="35" t="s">
         <v>74</v>
       </c>
-      <c r="N14" s="35"/>
-      <c r="O14" s="35"/>
-      <c r="P14" s="35"/>
+      <c r="N14" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="O14" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="P14" s="35" t="s">
+        <v>75</v>
+      </c>
       <c r="Q14" s="36"/>
       <c r="R14" s="76">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="S14" s="33" t="s">
         <v>71</v>
@@ -3168,18 +3275,26 @@
         <v>0.96052631578947367</v>
       </c>
       <c r="AA14" s="35"/>
-      <c r="AB14" s="35"/>
+      <c r="AB14" s="80">
+        <f>6/10</f>
+        <v>0.6</v>
+      </c>
       <c r="AC14" s="35"/>
       <c r="AD14" s="35"/>
       <c r="AE14" s="35"/>
       <c r="AF14" s="36"/>
-      <c r="AG14" s="59"/>
+      <c r="AG14" s="97">
+        <f t="shared" si="1"/>
+        <v>0.47502192982456143</v>
+      </c>
       <c r="AH14" s="59"/>
-      <c r="AI14" s="59"/>
-      <c r="AJ14" s="59"/>
-      <c r="AK14" s="59"/>
-      <c r="AL14" s="59"/>
-      <c r="AM14" s="59"/>
+      <c r="AI14" s="59" t="s">
+        <v>95</v>
+      </c>
+      <c r="AJ14" s="71"/>
+      <c r="AK14" s="71"/>
+      <c r="AL14" s="71"/>
+      <c r="AM14" s="71"/>
       <c r="AN14" s="59"/>
       <c r="AO14" s="59"/>
       <c r="AP14" s="59"/>
@@ -3273,18 +3388,24 @@
         <v>75</v>
       </c>
       <c r="L15" s="46" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="M15" s="46" t="s">
         <v>75</v>
       </c>
-      <c r="N15" s="46"/>
-      <c r="O15" s="46"/>
-      <c r="P15" s="46"/>
+      <c r="N15" s="46" t="s">
+        <v>74</v>
+      </c>
+      <c r="O15" s="46" t="s">
+        <v>75</v>
+      </c>
+      <c r="P15" s="46" t="s">
+        <v>75</v>
+      </c>
       <c r="Q15" s="47"/>
       <c r="R15" s="77">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="S15" s="44" t="s">
         <v>71</v>
@@ -3304,23 +3425,31 @@
         <v>0.9375</v>
       </c>
       <c r="Y15" s="85"/>
-      <c r="Z15" s="98">
+      <c r="Z15" s="91">
         <f>17.75/18</f>
         <v>0.98611111111111116</v>
       </c>
       <c r="AA15" s="46"/>
-      <c r="AB15" s="46"/>
+      <c r="AB15" s="81">
+        <f>7/10</f>
+        <v>0.7</v>
+      </c>
       <c r="AC15" s="46"/>
       <c r="AD15" s="46"/>
       <c r="AE15" s="46"/>
       <c r="AF15" s="47"/>
-      <c r="AG15" s="60"/>
+      <c r="AG15" s="97">
+        <f t="shared" si="1"/>
+        <v>0.50784722222222223</v>
+      </c>
       <c r="AH15" s="60"/>
-      <c r="AI15" s="60"/>
-      <c r="AJ15" s="60"/>
-      <c r="AK15" s="60"/>
-      <c r="AL15" s="60"/>
-      <c r="AM15" s="60"/>
+      <c r="AI15" s="60" t="s">
+        <v>86</v>
+      </c>
+      <c r="AJ15" s="94"/>
+      <c r="AK15" s="94"/>
+      <c r="AL15" s="94"/>
+      <c r="AM15" s="94"/>
       <c r="AN15" s="60"/>
       <c r="AO15" s="60"/>
       <c r="AP15" s="60"/>
@@ -3410,7 +3539,7 @@
       <c r="J16" s="35"/>
       <c r="K16" s="35"/>
       <c r="L16" s="35" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="M16" s="35" t="s">
         <v>74</v>
@@ -3441,19 +3570,27 @@
         <v>0.5625</v>
       </c>
       <c r="Y16" s="87"/>
-      <c r="Z16" s="97">
+      <c r="Z16" s="90">
         <f>7.25/18</f>
         <v>0.40277777777777779</v>
       </c>
       <c r="AA16" s="34"/>
-      <c r="AB16" s="35"/>
+      <c r="AB16" s="80">
+        <f>7/10</f>
+        <v>0.7</v>
+      </c>
       <c r="AC16" s="35"/>
       <c r="AD16" s="35"/>
       <c r="AE16" s="35"/>
       <c r="AF16" s="36"/>
-      <c r="AG16" s="59"/>
+      <c r="AG16" s="97">
+        <f t="shared" si="1"/>
+        <v>0.30159722222222224</v>
+      </c>
       <c r="AH16" s="59"/>
-      <c r="AI16" s="59"/>
+      <c r="AI16" s="59" t="s">
+        <v>87</v>
+      </c>
       <c r="AJ16" s="59"/>
       <c r="AK16" s="59"/>
       <c r="AL16" s="59"/>
@@ -3547,16 +3684,20 @@
       <c r="J17" s="35"/>
       <c r="K17" s="35"/>
       <c r="L17" s="35" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="M17" s="35"/>
-      <c r="N17" s="35"/>
-      <c r="O17" s="35"/>
+      <c r="N17" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="O17" s="35" t="s">
+        <v>75</v>
+      </c>
       <c r="P17" s="35"/>
       <c r="Q17" s="36"/>
       <c r="R17" s="76">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="S17" s="33"/>
       <c r="T17" s="34" t="s">
@@ -3569,24 +3710,32 @@
         <v>0.125</v>
       </c>
       <c r="W17" s="87"/>
-      <c r="X17" s="97">
+      <c r="X17" s="90">
         <f>2.5/8</f>
         <v>0.3125</v>
       </c>
-      <c r="Y17" s="99"/>
-      <c r="Z17" s="97">
+      <c r="Y17" s="92"/>
+      <c r="Z17" s="90">
         <f>6.5/18</f>
         <v>0.3611111111111111</v>
       </c>
       <c r="AA17" s="34"/>
-      <c r="AB17" s="35"/>
+      <c r="AB17" s="80">
+        <f>6/10</f>
+        <v>0.6</v>
+      </c>
       <c r="AC17" s="35"/>
       <c r="AD17" s="35"/>
       <c r="AE17" s="35"/>
       <c r="AF17" s="36"/>
-      <c r="AG17" s="59"/>
+      <c r="AG17" s="97">
+        <f t="shared" si="1"/>
+        <v>0.19159722222222222</v>
+      </c>
       <c r="AH17" s="59"/>
-      <c r="AI17" s="59"/>
+      <c r="AI17" s="59" t="s">
+        <v>88</v>
+      </c>
       <c r="AJ17" s="59"/>
       <c r="AK17" s="59"/>
       <c r="AL17" s="59"/>
@@ -3686,18 +3835,24 @@
         <v>74</v>
       </c>
       <c r="L18" s="35" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="M18" s="35" t="s">
         <v>74</v>
       </c>
-      <c r="N18" s="35"/>
-      <c r="O18" s="35"/>
-      <c r="P18" s="35"/>
+      <c r="N18" s="35" t="s">
+        <v>74</v>
+      </c>
+      <c r="O18" s="35" t="s">
+        <v>74</v>
+      </c>
+      <c r="P18" s="35" t="s">
+        <v>74</v>
+      </c>
       <c r="Q18" s="36"/>
       <c r="R18" s="76">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="S18" s="33" t="s">
         <v>71</v>
@@ -3721,14 +3876,22 @@
         <v>0.98611111111111116</v>
       </c>
       <c r="AA18" s="35"/>
-      <c r="AB18" s="35"/>
+      <c r="AB18" s="80">
+        <f>10/10</f>
+        <v>1</v>
+      </c>
       <c r="AC18" s="35"/>
       <c r="AD18" s="35"/>
       <c r="AE18" s="35"/>
       <c r="AF18" s="36"/>
-      <c r="AG18" s="59"/>
+      <c r="AG18" s="97">
+        <f t="shared" si="1"/>
+        <v>0.54722222222222228</v>
+      </c>
       <c r="AH18" s="59"/>
-      <c r="AI18" s="59"/>
+      <c r="AI18" s="59" t="s">
+        <v>89</v>
+      </c>
       <c r="AJ18" s="59"/>
       <c r="AK18" s="59"/>
       <c r="AL18" s="59"/>
@@ -3828,18 +3991,24 @@
         <v>74</v>
       </c>
       <c r="L19" s="46" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="M19" s="46" t="s">
         <v>74</v>
       </c>
-      <c r="N19" s="46"/>
-      <c r="O19" s="46"/>
-      <c r="P19" s="46"/>
+      <c r="N19" s="46" t="s">
+        <v>74</v>
+      </c>
+      <c r="O19" s="46" t="s">
+        <v>74</v>
+      </c>
+      <c r="P19" s="46" t="s">
+        <v>74</v>
+      </c>
       <c r="Q19" s="47"/>
       <c r="R19" s="77">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="S19" s="44" t="s">
         <v>0</v>
@@ -3863,14 +4032,22 @@
         <v>0.86111111111111116</v>
       </c>
       <c r="AA19" s="46"/>
-      <c r="AB19" s="46"/>
+      <c r="AB19" s="81">
+        <f>10/10</f>
+        <v>1</v>
+      </c>
       <c r="AC19" s="46"/>
       <c r="AD19" s="46"/>
       <c r="AE19" s="46"/>
       <c r="AF19" s="47"/>
-      <c r="AG19" s="60"/>
+      <c r="AG19" s="97">
+        <f t="shared" si="1"/>
+        <v>0.46597222222222223</v>
+      </c>
       <c r="AH19" s="60"/>
-      <c r="AI19" s="60"/>
+      <c r="AI19" s="60" t="s">
+        <v>96</v>
+      </c>
       <c r="AJ19" s="60"/>
       <c r="AK19" s="60"/>
       <c r="AL19" s="60"/>
@@ -3970,18 +4147,24 @@
         <v>75</v>
       </c>
       <c r="L20" s="56" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="M20" s="56" t="s">
         <v>75</v>
       </c>
-      <c r="N20" s="56"/>
-      <c r="O20" s="56"/>
-      <c r="P20" s="56"/>
+      <c r="N20" s="56" t="s">
+        <v>75</v>
+      </c>
+      <c r="O20" s="56" t="s">
+        <v>75</v>
+      </c>
+      <c r="P20" s="56" t="s">
+        <v>75</v>
+      </c>
       <c r="Q20" s="57"/>
       <c r="R20" s="76">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="S20" s="54"/>
       <c r="T20" s="55" t="s">
@@ -4003,12 +4186,18 @@
         <v>0.73684210526315785</v>
       </c>
       <c r="AA20" s="56"/>
-      <c r="AB20" s="56"/>
+      <c r="AB20" s="82">
+        <f>7/10</f>
+        <v>0.7</v>
+      </c>
       <c r="AC20" s="56"/>
       <c r="AD20" s="56"/>
       <c r="AE20" s="56"/>
       <c r="AF20" s="57"/>
-      <c r="AG20" s="59"/>
+      <c r="AG20" s="97">
+        <f t="shared" si="1"/>
+        <v>0.42361842105263159</v>
+      </c>
       <c r="AH20" s="59"/>
       <c r="AI20" s="59"/>
       <c r="AJ20" s="59"/>
@@ -4086,19 +4275,19 @@
       <c r="B21" s="72"/>
       <c r="C21" s="71"/>
       <c r="F21" s="72">
-        <f t="shared" ref="F21:I21" si="1">COUNTA(F4:F20)</f>
+        <f t="shared" ref="F21:I21" si="2">COUNTA(F4:F20)</f>
         <v>17</v>
       </c>
       <c r="G21" s="72">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>17</v>
       </c>
       <c r="H21" s="72">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>13</v>
       </c>
       <c r="I21" s="72">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>15</v>
       </c>
       <c r="J21" s="72">
@@ -4106,56 +4295,58 @@
         <v>13</v>
       </c>
       <c r="K21" s="72">
-        <f t="shared" ref="K21:Q21" si="2">COUNTA(K4:K20)</f>
+        <f t="shared" ref="K21:Q21" si="3">COUNTA(K4:K20)</f>
         <v>11</v>
       </c>
       <c r="L21" s="72">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>17</v>
       </c>
       <c r="M21" s="72">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>12</v>
       </c>
       <c r="N21" s="72">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
+        <v>14</v>
+      </c>
+      <c r="O21" s="72">
+        <f t="shared" si="3"/>
+        <v>12</v>
+      </c>
+      <c r="P21" s="72">
+        <f t="shared" si="3"/>
+        <v>11</v>
+      </c>
+      <c r="Q21" s="72">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="O21" s="72">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="P21" s="72">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="Q21" s="72">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
       <c r="R21" s="78"/>
-      <c r="S21" s="72"/>
+      <c r="S21" s="72" t="s">
+        <v>97</v>
+      </c>
       <c r="T21" s="72"/>
       <c r="U21" s="72"/>
-      <c r="V21" s="100">
+      <c r="V21" s="93">
         <v>0.1</v>
       </c>
       <c r="W21" s="72"/>
-      <c r="X21" s="100">
+      <c r="X21" s="93">
         <v>0.15</v>
       </c>
       <c r="Y21" s="72"/>
-      <c r="Z21" s="100">
+      <c r="Z21" s="93">
         <v>0.15</v>
       </c>
       <c r="AA21" s="72"/>
       <c r="AB21" s="72"/>
-      <c r="AC21" s="100">
+      <c r="AC21" s="93">
         <v>0.1</v>
       </c>
       <c r="AD21" s="72"/>
       <c r="AE21" s="72"/>
-      <c r="AF21" s="100">
+      <c r="AF21" s="93">
         <v>0.4</v>
       </c>
     </row>
@@ -4176,20 +4367,32 @@
       <c r="P22" s="72"/>
       <c r="Q22" s="72"/>
       <c r="R22" s="78"/>
-      <c r="S22" s="72"/>
+      <c r="S22" s="72" t="s">
+        <v>97</v>
+      </c>
       <c r="T22" s="72"/>
       <c r="U22" s="72"/>
-      <c r="V22" s="72"/>
-      <c r="W22" s="72"/>
-      <c r="X22" s="72"/>
-      <c r="Y22" s="72"/>
-      <c r="Z22" s="72"/>
-      <c r="AA22" s="72"/>
-      <c r="AB22" s="72"/>
-      <c r="AC22" s="72"/>
-      <c r="AD22" s="72"/>
-      <c r="AE22" s="72"/>
-      <c r="AF22" s="72"/>
+      <c r="V22" s="95">
+        <v>0.1</v>
+      </c>
+      <c r="W22" s="95"/>
+      <c r="X22" s="95">
+        <v>0.15</v>
+      </c>
+      <c r="Y22" s="95"/>
+      <c r="Z22" s="95">
+        <v>0.2</v>
+      </c>
+      <c r="AA22" s="95"/>
+      <c r="AB22" s="95"/>
+      <c r="AC22" s="95">
+        <v>0.1</v>
+      </c>
+      <c r="AD22" s="95"/>
+      <c r="AE22" s="95"/>
+      <c r="AF22" s="95">
+        <v>0.45</v>
+      </c>
     </row>
     <row r="23" spans="1:104" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="71"/>
@@ -4208,14 +4411,25 @@
       <c r="P23" s="72"/>
       <c r="Q23" s="72"/>
       <c r="R23" s="78"/>
-      <c r="S23" s="72"/>
+      <c r="S23" s="72" t="s">
+        <v>98</v>
+      </c>
       <c r="T23" s="72"/>
       <c r="U23" s="72"/>
-      <c r="V23" s="72"/>
+      <c r="V23" s="95">
+        <f>SUM(V4:V20)/17</f>
+        <v>0.84199346405228759</v>
+      </c>
       <c r="W23" s="72"/>
-      <c r="X23" s="72"/>
+      <c r="X23" s="95">
+        <f>SUM(X4:X20)/17</f>
+        <v>0.78492647058823528</v>
+      </c>
       <c r="Y23" s="72"/>
-      <c r="Z23" s="72"/>
+      <c r="Z23" s="95">
+        <f>SUM(Z4:Z20)/17</f>
+        <v>0.72015823873409013</v>
+      </c>
       <c r="AA23" s="72"/>
       <c r="AB23" s="72"/>
       <c r="AC23" s="72"/>
@@ -5056,6 +5270,11 @@
       <c r="CZ41" s="59"/>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="AG4:AG20">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
+      <formula>0.4</formula>
+    </cfRule>
+  </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="C32" r:id="rId1" xr:uid="{31ADC0CD-3FE5-43AB-B1AE-625F8CE4B16F}"/>
     <hyperlink ref="C34" r:id="rId2" xr:uid="{9E5FE872-B605-4C45-8564-4F6553F9811E}"/>

</xml_diff>